<commit_message>
"Made the login page"
</commit_message>
<xml_diff>
--- a/data/station_data.xlsx
+++ b/data/station_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education\Internships\Railway\prototype\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Education\Internships\Railway\prototype\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC411431-E164-4C79-8578-97A36F0F6A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B5737B-6BB6-4CA1-82F0-323D165F8E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="587">
   <si>
     <t>Station Code</t>
   </si>
@@ -1781,15 +1781,6 @@
   </si>
   <si>
     <t>Titabar</t>
-  </si>
-  <si>
-    <t>﻿25.806579</t>
-  </si>
-  <si>
-    <t>﻿26.1507</t>
-  </si>
-  <si>
-    <t>﻿26.692778</t>
   </si>
 </sst>
 </file>
@@ -2159,14 +2150,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
-      <selection activeCell="F280" sqref="F280"/>
+    <sheetView tabSelected="1" topLeftCell="A253" workbookViewId="0">
+      <selection activeCell="G247" sqref="G247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="27.81640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -2199,10 +2187,10 @@
         <v>309</v>
       </c>
       <c r="D2">
-        <v>24.977049999999998</v>
+        <v>25.288599999999999</v>
       </c>
       <c r="E2">
-        <v>88.156700000000001</v>
+        <v>88.383669999999995</v>
       </c>
       <c r="F2">
         <v>732128</v>
@@ -2219,10 +2207,10 @@
         <v>310</v>
       </c>
       <c r="D3">
-        <v>26.131138</v>
+        <v>26.133849000000001</v>
       </c>
       <c r="E3">
-        <v>87.445533999999995</v>
+        <v>87.466819000000001</v>
       </c>
       <c r="F3">
         <v>854311</v>
@@ -2238,12 +2226,6 @@
       <c r="C4" t="s">
         <v>311</v>
       </c>
-      <c r="D4">
-        <v>26.136199999999999</v>
-      </c>
-      <c r="E4">
-        <v>87.412499999999994</v>
-      </c>
       <c r="F4">
         <v>854321</v>
       </c>
@@ -2259,10 +2241,10 @@
         <v>312</v>
       </c>
       <c r="D5">
-        <v>26.269042800000001</v>
+        <v>25.25</v>
       </c>
       <c r="E5">
-        <v>88.185246800000002</v>
+        <v>88.19</v>
       </c>
       <c r="F5">
         <v>733202</v>
@@ -2279,10 +2261,10 @@
         <v>313</v>
       </c>
       <c r="D6">
-        <v>25.671579999999999</v>
+        <v>26.2302553</v>
       </c>
       <c r="E6">
-        <v>88.192850000000007</v>
+        <v>88.771419499999993</v>
       </c>
       <c r="F6">
         <v>733134</v>
@@ -2299,10 +2281,10 @@
         <v>314</v>
       </c>
       <c r="D7">
-        <v>25.331399999999999</v>
+        <v>25.415777800000001</v>
       </c>
       <c r="E7">
-        <v>87.922899999999998</v>
+        <v>87.875222199999996</v>
       </c>
       <c r="F7">
         <v>732125</v>
@@ -2319,10 +2301,10 @@
         <v>315</v>
       </c>
       <c r="D8">
-        <v>25.385999999999999</v>
+        <v>25.396409999999999</v>
       </c>
       <c r="E8">
-        <v>88.4011</v>
+        <v>88.423349999999999</v>
       </c>
       <c r="F8">
         <v>733121</v>
@@ -2339,10 +2321,10 @@
         <v>316</v>
       </c>
       <c r="D9">
-        <v>25.6509</v>
+        <v>25.537500000000001</v>
       </c>
       <c r="E9">
-        <v>87.922600000000003</v>
+        <v>87.566000000000003</v>
       </c>
       <c r="F9">
         <v>854317</v>
@@ -2359,10 +2341,10 @@
         <v>317</v>
       </c>
       <c r="D10">
-        <v>26.6983</v>
+        <v>26.6998611</v>
       </c>
       <c r="E10">
-        <v>88.324399999999997</v>
+        <v>88.313916699999993</v>
       </c>
       <c r="F10">
         <v>734014</v>
@@ -2379,10 +2361,10 @@
         <v>318</v>
       </c>
       <c r="D11">
-        <v>26.651593999999999</v>
+        <v>26.537334000000001</v>
       </c>
       <c r="E11">
-        <v>85.576644999999999</v>
+        <v>85.495213000000007</v>
       </c>
       <c r="F11">
         <v>843322</v>
@@ -2399,10 +2381,10 @@
         <v>319</v>
       </c>
       <c r="D12">
-        <v>26.54908</v>
+        <v>22.5839167</v>
       </c>
       <c r="E12">
-        <v>88.323779999999999</v>
+        <v>88.308833300000003</v>
       </c>
       <c r="F12">
         <v>711104</v>
@@ -2419,10 +2401,10 @@
         <v>320</v>
       </c>
       <c r="D13">
-        <v>25.611799999999999</v>
+        <v>25.473109999999998</v>
       </c>
       <c r="E13">
-        <v>87.560850000000002</v>
+        <v>87.432400000000001</v>
       </c>
       <c r="F13">
         <v>854106</v>
@@ -2439,10 +2421,10 @@
         <v>321</v>
       </c>
       <c r="D14">
-        <v>25.873999999999999</v>
+        <v>25.890833300000001</v>
       </c>
       <c r="E14">
-        <v>87.838999999999999</v>
+        <v>87.840555499999994</v>
       </c>
       <c r="F14">
         <v>733201</v>
@@ -2459,10 +2441,10 @@
         <v>322</v>
       </c>
       <c r="D15">
-        <v>25.32611</v>
+        <v>23.617977</v>
       </c>
       <c r="E15">
-        <v>88.332790000000003</v>
+        <v>87.116152999999997</v>
       </c>
       <c r="F15">
         <v>713347</v>
@@ -2479,10 +2461,10 @@
         <v>323</v>
       </c>
       <c r="D16">
-        <v>25.640363000000001</v>
+        <v>25.6782222</v>
       </c>
       <c r="E16">
-        <v>88.386474100000001</v>
+        <v>88.333277800000005</v>
       </c>
       <c r="F16">
         <v>733129</v>
@@ -2499,10 +2481,10 @@
         <v>324</v>
       </c>
       <c r="D17">
-        <v>26.476900000000001</v>
+        <v>26.31</v>
       </c>
       <c r="E17">
-        <v>88.296099999999996</v>
+        <v>88.28</v>
       </c>
       <c r="F17">
         <v>733207</v>
@@ -2519,10 +2501,10 @@
         <v>325</v>
       </c>
       <c r="D18">
-        <v>25.574069999999999</v>
+        <v>25.537500000000001</v>
       </c>
       <c r="E18">
-        <v>87.647059999999996</v>
+        <v>87.566000000000003</v>
       </c>
       <c r="F18">
         <v>855114</v>
@@ -2539,10 +2521,10 @@
         <v>326</v>
       </c>
       <c r="D19">
-        <v>25.170308299999999</v>
+        <v>25.015555599999999</v>
       </c>
       <c r="E19">
-        <v>88.101209900000001</v>
+        <v>88.132361099999997</v>
       </c>
       <c r="F19">
         <v>732102</v>
@@ -2559,10 +2541,10 @@
         <v>327</v>
       </c>
       <c r="D20">
-        <v>26.2989</v>
+        <v>26.307994000000001</v>
       </c>
       <c r="E20">
-        <v>87.262100000000004</v>
+        <v>87.260808999999995</v>
       </c>
       <c r="F20">
         <v>854318</v>
@@ -2579,10 +2561,10 @@
         <v>328</v>
       </c>
       <c r="D21">
-        <v>26.52826</v>
+        <v>25.678159999999998</v>
       </c>
       <c r="E21">
-        <v>88.112700000000004</v>
+        <v>86.941142999999997</v>
       </c>
       <c r="F21">
         <v>855106</v>
@@ -2599,10 +2581,10 @@
         <v>329</v>
       </c>
       <c r="D22">
-        <v>26.184480000000001</v>
+        <v>25.25</v>
       </c>
       <c r="E22">
-        <v>88.090010000000007</v>
+        <v>88.19</v>
       </c>
       <c r="F22">
         <v>733202</v>
@@ -2619,10 +2601,10 @@
         <v>330</v>
       </c>
       <c r="D23">
-        <v>25.390499999999999</v>
+        <v>25.3968889</v>
       </c>
       <c r="E23">
-        <v>88.517499999999998</v>
+        <v>88.514611099999996</v>
       </c>
       <c r="F23">
         <v>733124</v>
@@ -2639,10 +2621,10 @@
         <v>331</v>
       </c>
       <c r="D24">
-        <v>25.404</v>
+        <v>25.415777800000001</v>
       </c>
       <c r="E24">
-        <v>87.868499999999997</v>
+        <v>87.875222199999996</v>
       </c>
       <c r="F24">
         <v>732125</v>
@@ -2659,10 +2641,10 @@
         <v>332</v>
       </c>
       <c r="D25">
-        <v>23.310863000000001</v>
+        <v>25.8738888</v>
       </c>
       <c r="E25">
-        <v>85.307158999999999</v>
+        <v>87.840277700000001</v>
       </c>
       <c r="F25">
         <v>733209</v>
@@ -2679,10 +2661,10 @@
         <v>333</v>
       </c>
       <c r="D26">
-        <v>25.952985200000001</v>
+        <v>25.960965000000002</v>
       </c>
       <c r="E26">
-        <v>87.5299634</v>
+        <v>87.509906000000001</v>
       </c>
       <c r="F26">
         <v>854327</v>
@@ -2699,10 +2681,10 @@
         <v>334</v>
       </c>
       <c r="D27">
-        <v>26.4026</v>
+        <v>26.36411</v>
       </c>
       <c r="E27">
-        <v>87.2637</v>
+        <v>87.276753999999997</v>
       </c>
       <c r="F27">
         <v>854328</v>
@@ -2719,10 +2701,10 @@
         <v>335</v>
       </c>
       <c r="D28">
-        <v>26.518699999999999</v>
+        <v>26.700638900000001</v>
       </c>
       <c r="E28">
-        <v>88.724100000000007</v>
+        <v>88.433166700000001</v>
       </c>
       <c r="F28">
         <v>734004</v>
@@ -2739,10 +2721,10 @@
         <v>336</v>
       </c>
       <c r="D29">
-        <v>25.638999999999999</v>
+        <v>25.6782222</v>
       </c>
       <c r="E29">
-        <v>88.327500000000001</v>
+        <v>88.333277800000005</v>
       </c>
       <c r="F29">
         <v>733129</v>
@@ -2759,10 +2741,10 @@
         <v>337</v>
       </c>
       <c r="D30">
-        <v>25.635819999999999</v>
+        <v>25.537500000000001</v>
       </c>
       <c r="E30">
-        <v>88.019270000000006</v>
+        <v>87.566000000000003</v>
       </c>
       <c r="F30">
         <v>854317</v>
@@ -2779,10 +2761,10 @@
         <v>338</v>
       </c>
       <c r="D31">
-        <v>25.427499999999998</v>
+        <v>25.415777800000001</v>
       </c>
       <c r="E31">
-        <v>87.807299999999998</v>
+        <v>87.875222199999996</v>
       </c>
       <c r="F31">
         <v>732125</v>
@@ -2799,10 +2781,10 @@
         <v>339</v>
       </c>
       <c r="D32">
-        <v>25.547999999999998</v>
+        <v>25.537099999999999</v>
       </c>
       <c r="E32">
-        <v>87.565200000000004</v>
+        <v>87.575999999999993</v>
       </c>
       <c r="F32">
         <v>854105</v>
@@ -2819,10 +2801,10 @@
         <v>340</v>
       </c>
       <c r="D33">
-        <v>26.003233000000002</v>
+        <v>25.8738888</v>
       </c>
       <c r="E33">
-        <v>87.864524000000003</v>
+        <v>87.840277700000001</v>
       </c>
       <c r="F33">
         <v>733209</v>
@@ -2839,10 +2821,10 @@
         <v>341</v>
       </c>
       <c r="D34">
-        <v>26.546419</v>
+        <v>26.237203000000001</v>
       </c>
       <c r="E34">
-        <v>81.841117999999994</v>
+        <v>89.485219000000001</v>
       </c>
       <c r="F34">
         <v>736134</v>
@@ -2859,10 +2841,10 @@
         <v>342</v>
       </c>
       <c r="D35">
-        <v>26.307793</v>
+        <v>26.312806999999999</v>
       </c>
       <c r="E35">
-        <v>87.776336999999998</v>
+        <v>87.758139</v>
       </c>
       <c r="F35">
         <v>855107</v>
@@ -2879,10 +2861,10 @@
         <v>343</v>
       </c>
       <c r="D36">
-        <v>25.486219999999999</v>
+        <v>25.537500000000001</v>
       </c>
       <c r="E36">
-        <v>87.705860000000001</v>
+        <v>87.566000000000003</v>
       </c>
       <c r="F36">
         <v>854103</v>
@@ -2899,10 +2881,10 @@
         <v>344</v>
       </c>
       <c r="D37">
-        <v>26.157250000000001</v>
+        <v>26.056822</v>
       </c>
       <c r="E37">
-        <v>87.463099999999997</v>
+        <v>87.589009000000004</v>
       </c>
       <c r="F37">
         <v>854325</v>
@@ -2919,10 +2901,10 @@
         <v>345</v>
       </c>
       <c r="D38">
-        <v>22.517617999999999</v>
+        <v>22.572777800000001</v>
       </c>
       <c r="E38">
-        <v>88.384048000000007</v>
+        <v>88.347499999999997</v>
       </c>
       <c r="F38">
         <v>700042</v>
@@ -2939,10 +2921,10 @@
         <v>346</v>
       </c>
       <c r="D39">
-        <v>25.490641100000001</v>
+        <v>25.3215</v>
       </c>
       <c r="E39">
-        <v>87.826798100000005</v>
+        <v>87.335700000000003</v>
       </c>
       <c r="F39">
         <v>855113</v>
@@ -2959,10 +2941,10 @@
         <v>347</v>
       </c>
       <c r="D40">
-        <v>25.439810000000001</v>
+        <v>25.544194399999999</v>
       </c>
       <c r="E40">
-        <v>87.744600000000005</v>
+        <v>87.569833299999999</v>
       </c>
       <c r="F40">
         <v>854116</v>
@@ -2979,10 +2961,10 @@
         <v>348</v>
       </c>
       <c r="D41">
-        <v>25.629245000000001</v>
+        <v>25.3215</v>
       </c>
       <c r="E41">
-        <v>87.887152999999998</v>
+        <v>87.335700000000003</v>
       </c>
       <c r="F41">
         <v>855113</v>
@@ -2999,10 +2981,10 @@
         <v>349</v>
       </c>
       <c r="D42">
-        <v>25.486219999999999</v>
+        <v>25.537500000000001</v>
       </c>
       <c r="E42">
-        <v>87.705860000000001</v>
+        <v>87.566000000000003</v>
       </c>
       <c r="F42">
         <v>854103</v>
@@ -3019,10 +3001,10 @@
         <v>350</v>
       </c>
       <c r="D43">
-        <v>26.412489999999998</v>
+        <v>25.678159999999998</v>
       </c>
       <c r="E43">
-        <v>88.256910000000005</v>
+        <v>86.941142999999997</v>
       </c>
       <c r="F43">
         <v>855117</v>
@@ -3039,10 +3021,10 @@
         <v>351</v>
       </c>
       <c r="D44">
-        <v>26.6798</v>
+        <v>26.6823035</v>
       </c>
       <c r="E44">
-        <v>88.198400000000007</v>
+        <v>88.199851199999998</v>
       </c>
       <c r="F44">
         <v>734429</v>
@@ -3059,10 +3041,10 @@
         <v>352</v>
       </c>
       <c r="D45">
-        <v>26.684200000000001</v>
+        <v>26.684472199999998</v>
       </c>
       <c r="E45">
-        <v>88.442800000000005</v>
+        <v>88.421194400000005</v>
       </c>
       <c r="F45">
         <v>734007</v>
@@ -3079,10 +3061,10 @@
         <v>353</v>
       </c>
       <c r="D46">
-        <v>25.0533</v>
+        <v>24.9980555</v>
       </c>
       <c r="E46">
-        <v>88.1434</v>
+        <v>88.137777700000001</v>
       </c>
       <c r="F46">
         <v>732128</v>
@@ -3099,10 +3081,10 @@
         <v>354</v>
       </c>
       <c r="D47">
-        <v>26.139416300000001</v>
+        <v>26.144166599999998</v>
       </c>
       <c r="E47">
-        <v>88.016991000000004</v>
+        <v>88.026944400000005</v>
       </c>
       <c r="F47">
         <v>733208</v>
@@ -3119,10 +3101,10 @@
         <v>355</v>
       </c>
       <c r="D48">
-        <v>25.4620663</v>
+        <v>25.544194399999999</v>
       </c>
       <c r="E48">
-        <v>87.704341200000002</v>
+        <v>87.569833299999999</v>
       </c>
       <c r="F48">
         <v>854116</v>
@@ -3139,10 +3121,10 @@
         <v>356</v>
       </c>
       <c r="D49">
-        <v>25.789100000000001</v>
+        <v>25.771435</v>
       </c>
       <c r="E49">
-        <v>87.519199999999998</v>
+        <v>87.471035000000001</v>
       </c>
       <c r="F49">
         <v>854301</v>
@@ -3159,10 +3141,10 @@
         <v>357</v>
       </c>
       <c r="D50">
-        <v>25.643115699999999</v>
+        <v>25.6782222</v>
       </c>
       <c r="E50">
-        <v>88.447793399999995</v>
+        <v>88.333277800000005</v>
       </c>
       <c r="F50">
         <v>733129</v>
@@ -3179,10 +3161,10 @@
         <v>358</v>
       </c>
       <c r="D51">
-        <v>25.6189</v>
+        <v>26.2302553</v>
       </c>
       <c r="E51">
-        <v>88.128900000000002</v>
+        <v>88.771419499999993</v>
       </c>
       <c r="F51">
         <v>733134</v>
@@ -3199,10 +3181,10 @@
         <v>359</v>
       </c>
       <c r="D52">
-        <v>26.665099999999999</v>
+        <v>25.692499999999999</v>
       </c>
       <c r="E52">
-        <v>88.375799999999998</v>
+        <v>88.384444400000007</v>
       </c>
       <c r="F52">
         <v>734434</v>
@@ -3219,10 +3201,10 @@
         <v>360</v>
       </c>
       <c r="D53">
-        <v>26.543900000000001</v>
+        <v>26.55</v>
       </c>
       <c r="E53">
-        <v>88.648200000000003</v>
+        <v>88.71</v>
       </c>
       <c r="F53">
         <v>735121</v>
@@ -3259,10 +3241,10 @@
         <v>362</v>
       </c>
       <c r="D55">
-        <v>26.723700000000001</v>
+        <v>26.712861100000001</v>
       </c>
       <c r="E55">
-        <v>88.413899999999998</v>
+        <v>88.424499999999995</v>
       </c>
       <c r="F55">
         <v>734001</v>
@@ -3279,10 +3261,10 @@
         <v>363</v>
       </c>
       <c r="D56">
-        <v>26.706</v>
+        <v>26.700638900000001</v>
       </c>
       <c r="E56">
-        <v>88.430300000000003</v>
+        <v>88.433166700000001</v>
       </c>
       <c r="F56">
         <v>734004</v>
@@ -3299,10 +3281,10 @@
         <v>364</v>
       </c>
       <c r="D57">
-        <v>25.935929999999999</v>
+        <v>25.8738888</v>
       </c>
       <c r="E57">
-        <v>87.849260000000001</v>
+        <v>87.840277700000001</v>
       </c>
       <c r="F57">
         <v>733209</v>
@@ -3319,10 +3301,10 @@
         <v>365</v>
       </c>
       <c r="D58">
-        <v>26.274957000000001</v>
+        <v>26.307994000000001</v>
       </c>
       <c r="E58">
-        <v>87.241929999999996</v>
+        <v>87.260808999999995</v>
       </c>
       <c r="F58">
         <v>854318</v>
@@ -3339,10 +3321,10 @@
         <v>366</v>
       </c>
       <c r="D59">
-        <v>25.6157</v>
+        <v>25.3215</v>
       </c>
       <c r="E59">
-        <v>87.837500000000006</v>
+        <v>87.335700000000003</v>
       </c>
       <c r="F59">
         <v>855113</v>
@@ -3359,10 +3341,10 @@
         <v>367</v>
       </c>
       <c r="D60">
-        <v>25.727854000000001</v>
+        <v>25.537500000000001</v>
       </c>
       <c r="E60">
-        <v>87.879489000000007</v>
+        <v>87.566000000000003</v>
       </c>
       <c r="F60">
         <v>854317</v>
@@ -3378,11 +3360,11 @@
       <c r="C61" t="s">
         <v>368</v>
       </c>
-      <c r="D61" t="s">
-        <v>587</v>
+      <c r="D61">
+        <v>25.537500000000001</v>
       </c>
       <c r="E61">
-        <v>87.842209999999994</v>
+        <v>87.566000000000003</v>
       </c>
       <c r="F61">
         <v>854317</v>
@@ -3399,10 +3381,10 @@
         <v>369</v>
       </c>
       <c r="D62">
-        <v>26.428100000000001</v>
+        <v>26.419888799999999</v>
       </c>
       <c r="E62">
-        <v>88.128699999999995</v>
+        <v>88.131694400000001</v>
       </c>
       <c r="F62">
         <v>855116</v>
@@ -3419,10 +3401,10 @@
         <v>370</v>
       </c>
       <c r="D63">
-        <v>26.478999999999999</v>
+        <v>26.530805600000001</v>
       </c>
       <c r="E63">
-        <v>89.521000000000001</v>
+        <v>89.539138899999998</v>
       </c>
       <c r="F63">
         <v>736123</v>
@@ -3439,10 +3421,10 @@
         <v>371</v>
       </c>
       <c r="D64">
-        <v>26.491890000000001</v>
+        <v>26.530805600000001</v>
       </c>
       <c r="E64">
-        <v>89.527100000000004</v>
+        <v>89.539138899999998</v>
       </c>
       <c r="F64">
         <v>736123</v>
@@ -3459,10 +3441,10 @@
         <v>372</v>
       </c>
       <c r="D65">
-        <v>26.788139999999999</v>
+        <v>26.79</v>
       </c>
       <c r="E65">
-        <v>89.040800000000004</v>
+        <v>89.03</v>
       </c>
       <c r="F65">
         <v>735202</v>
@@ -3479,10 +3461,10 @@
         <v>373</v>
       </c>
       <c r="D66">
-        <v>26.747199999999999</v>
+        <v>26.76</v>
       </c>
       <c r="E66">
-        <v>89.053799999999995</v>
+        <v>89.06</v>
       </c>
       <c r="F66">
         <v>735232</v>
@@ -3499,10 +3481,10 @@
         <v>374</v>
       </c>
       <c r="D67">
-        <v>26.8705</v>
+        <v>26.89</v>
       </c>
       <c r="E67">
-        <v>88.585599999999999</v>
+        <v>88.57</v>
       </c>
       <c r="F67">
         <v>734501</v>
@@ -3519,10 +3501,10 @@
         <v>375</v>
       </c>
       <c r="D68">
-        <v>26.4600446</v>
+        <v>26.466699999999999</v>
       </c>
       <c r="E68">
-        <v>90.419481599999997</v>
+        <v>90.4</v>
       </c>
       <c r="F68">
         <v>783372</v>
@@ -3539,10 +3521,10 @@
         <v>376</v>
       </c>
       <c r="D69">
-        <v>26.388200000000001</v>
+        <v>26.397500000000001</v>
       </c>
       <c r="E69">
-        <v>89.494470000000007</v>
+        <v>89.498333299999999</v>
       </c>
       <c r="F69">
         <v>736133</v>
@@ -3562,7 +3544,7 @@
         <v>26.88</v>
       </c>
       <c r="E70">
-        <v>88.78</v>
+        <v>88.81</v>
       </c>
       <c r="F70">
         <v>735206</v>
@@ -3579,10 +3561,10 @@
         <v>378</v>
       </c>
       <c r="D71">
-        <v>26.401900000000001</v>
+        <v>26.335833300000001</v>
       </c>
       <c r="E71">
-        <v>90.085800000000006</v>
+        <v>90.111194400000002</v>
       </c>
       <c r="F71">
         <v>783337</v>
@@ -3598,11 +3580,11 @@
       <c r="C72" t="s">
         <v>379</v>
       </c>
-      <c r="D72" t="s">
-        <v>588</v>
+      <c r="D72">
+        <v>26.018694400000001</v>
       </c>
       <c r="E72">
-        <v>90.086399999999998</v>
+        <v>89.994277800000006</v>
       </c>
       <c r="F72">
         <v>783301</v>
@@ -3619,10 +3601,10 @@
         <v>380</v>
       </c>
       <c r="D73">
-        <v>26.865600000000001</v>
+        <v>26.85</v>
       </c>
       <c r="E73">
-        <v>88.669799999999995</v>
+        <v>88.67</v>
       </c>
       <c r="F73">
         <v>735209</v>
@@ -3639,10 +3621,10 @@
         <v>381</v>
       </c>
       <c r="D74">
-        <v>26.714700000000001</v>
+        <v>26.556408000000001</v>
       </c>
       <c r="E74">
-        <v>89.136799999999994</v>
+        <v>92.200734800000006</v>
       </c>
       <c r="F74">
         <v>784116</v>
@@ -3659,10 +3641,10 @@
         <v>382</v>
       </c>
       <c r="D75">
-        <v>26.574200000000001</v>
+        <v>26.59</v>
       </c>
       <c r="E75">
-        <v>88.993899999999996</v>
+        <v>89.01</v>
       </c>
       <c r="F75">
         <v>735210</v>
@@ -3679,10 +3661,10 @@
         <v>383</v>
       </c>
       <c r="D76">
-        <v>26.36524</v>
+        <v>26.364599999999999</v>
       </c>
       <c r="E76">
-        <v>90.186189999999996</v>
+        <v>90.183400000000006</v>
       </c>
       <c r="F76">
         <v>783345</v>
@@ -3699,10 +3681,10 @@
         <v>384</v>
       </c>
       <c r="D77">
-        <v>26.4224</v>
+        <v>26.425555500000002</v>
       </c>
       <c r="E77">
-        <v>89.277799999999999</v>
+        <v>89.276388800000007</v>
       </c>
       <c r="F77">
         <v>736171</v>
@@ -3719,10 +3701,10 @@
         <v>385</v>
       </c>
       <c r="D78">
-        <v>26.108000000000001</v>
+        <v>26.1058889</v>
       </c>
       <c r="E78">
-        <v>89.830799999999996</v>
+        <v>89.824388900000002</v>
       </c>
       <c r="F78">
         <v>783334</v>
@@ -3739,10 +3721,10 @@
         <v>386</v>
       </c>
       <c r="D79">
-        <v>26.803059999999999</v>
+        <v>26.789483000000001</v>
       </c>
       <c r="E79">
-        <v>88.404409999999999</v>
+        <v>88.363714000000002</v>
       </c>
       <c r="F79">
         <v>734009</v>
@@ -3759,10 +3741,10 @@
         <v>387</v>
       </c>
       <c r="D80">
-        <v>26.429600000000001</v>
+        <v>26.438055599999998</v>
       </c>
       <c r="E80">
-        <v>89.976900000000001</v>
+        <v>89.979916700000004</v>
       </c>
       <c r="F80">
         <v>783360</v>
@@ -3779,10 +3761,10 @@
         <v>388</v>
       </c>
       <c r="D81">
-        <v>26.077200000000001</v>
+        <v>26.085777799999999</v>
       </c>
       <c r="E81">
-        <v>89.955600000000004</v>
+        <v>89.9656667</v>
       </c>
       <c r="F81">
         <v>783331</v>
@@ -3799,10 +3781,10 @@
         <v>389</v>
       </c>
       <c r="D82">
-        <v>26.730899999999998</v>
+        <v>26.735638900000001</v>
       </c>
       <c r="E82">
-        <v>89.3506</v>
+        <v>89.365750000000006</v>
       </c>
       <c r="F82">
         <v>735215</v>
@@ -3819,10 +3801,10 @@
         <v>390</v>
       </c>
       <c r="D83">
-        <v>26.456099999999999</v>
+        <v>26.470486000000001</v>
       </c>
       <c r="E83">
-        <v>89.8048</v>
+        <v>89.805122999999995</v>
       </c>
       <c r="F83">
         <v>736207</v>
@@ -3839,10 +3821,10 @@
         <v>391</v>
       </c>
       <c r="D84">
-        <v>26.5593182</v>
+        <v>26.55</v>
       </c>
       <c r="E84">
-        <v>88.709275399999996</v>
+        <v>88.71</v>
       </c>
       <c r="F84">
         <v>735121</v>
@@ -3859,10 +3841,10 @@
         <v>392</v>
       </c>
       <c r="D85">
-        <v>26.481636000000002</v>
+        <v>26.471074999999999</v>
       </c>
       <c r="E85">
-        <v>89.732894999999999</v>
+        <v>89.726094000000003</v>
       </c>
       <c r="F85">
         <v>736202</v>
@@ -3878,11 +3860,11 @@
       <c r="C86" t="s">
         <v>393</v>
       </c>
-      <c r="D86" t="s">
-        <v>589</v>
+      <c r="D86">
+        <v>26.693055600000001</v>
       </c>
       <c r="E86">
-        <v>89.471666999999997</v>
+        <v>89.445499999999996</v>
       </c>
       <c r="F86">
         <v>735217</v>
@@ -3899,10 +3881,10 @@
         <v>394</v>
       </c>
       <c r="D87">
-        <v>26.401436</v>
+        <v>26.403694399999999</v>
       </c>
       <c r="E87">
-        <v>90.266700999999998</v>
+        <v>90.272194400000004</v>
       </c>
       <c r="F87">
         <v>783370</v>
@@ -3919,10 +3901,10 @@
         <v>395</v>
       </c>
       <c r="D88">
-        <v>26.7057</v>
+        <v>26.7</v>
       </c>
       <c r="E88">
-        <v>88.7697</v>
+        <v>88.7</v>
       </c>
       <c r="F88">
         <v>735219</v>
@@ -3939,10 +3921,10 @@
         <v>396</v>
       </c>
       <c r="D89">
-        <v>26.8659</v>
+        <v>26.86</v>
       </c>
       <c r="E89">
-        <v>88.737499999999997</v>
+        <v>88.74</v>
       </c>
       <c r="F89">
         <v>735221</v>
@@ -3959,10 +3941,10 @@
         <v>397</v>
       </c>
       <c r="D90">
-        <v>27.18</v>
+        <v>27.105699999999999</v>
       </c>
       <c r="E90">
-        <v>95.33</v>
+        <v>95.212699999999998</v>
       </c>
       <c r="F90">
         <v>786621</v>
@@ -3979,10 +3961,10 @@
         <v>398</v>
       </c>
       <c r="D91">
-        <v>27.650722399999999</v>
+        <v>26.397500000000001</v>
       </c>
       <c r="E91">
-        <v>85.411077399999996</v>
+        <v>89.498333299999999</v>
       </c>
       <c r="F91">
         <v>736133</v>
@@ -3999,10 +3981,10 @@
         <v>399</v>
       </c>
       <c r="D92">
-        <v>26.323920999999999</v>
+        <v>26.325821000000001</v>
       </c>
       <c r="E92">
-        <v>89.451087999999999</v>
+        <v>89.460526000000002</v>
       </c>
       <c r="F92">
         <v>736101</v>
@@ -4019,10 +4001,10 @@
         <v>400</v>
       </c>
       <c r="D93">
-        <v>22.882218999999999</v>
+        <v>26.98</v>
       </c>
       <c r="E93">
-        <v>88.014420000000001</v>
+        <v>88.92</v>
       </c>
       <c r="F93">
         <v>735225</v>
@@ -4039,10 +4021,10 @@
         <v>401</v>
       </c>
       <c r="D94">
-        <v>26.573830000000001</v>
+        <v>26.56</v>
       </c>
       <c r="E94">
-        <v>88.821494999999999</v>
+        <v>88.82</v>
       </c>
       <c r="F94">
         <v>735224</v>
@@ -4059,10 +4041,10 @@
         <v>402</v>
       </c>
       <c r="D95">
-        <v>17.762419999999999</v>
+        <v>26.86</v>
       </c>
       <c r="E95">
-        <v>73.195459999999997</v>
+        <v>88.74</v>
       </c>
       <c r="F95">
         <v>735221</v>
@@ -4079,10 +4061,10 @@
         <v>403</v>
       </c>
       <c r="D96">
-        <v>26.491890000000001</v>
+        <v>26.530805600000001</v>
       </c>
       <c r="E96">
-        <v>89.527100000000004</v>
+        <v>89.539138899999998</v>
       </c>
       <c r="F96">
         <v>736123</v>
@@ -4099,10 +4081,10 @@
         <v>404</v>
       </c>
       <c r="D97">
-        <v>26.422171299999999</v>
+        <v>26.5763888</v>
       </c>
       <c r="E97">
-        <v>89.352186500000002</v>
+        <v>89.382499999999993</v>
       </c>
       <c r="F97">
         <v>736165</v>
@@ -4119,10 +4101,10 @@
         <v>405</v>
       </c>
       <c r="D98">
-        <v>26.441438600000001</v>
+        <v>26.401399999999999</v>
       </c>
       <c r="E98">
-        <v>90.314282500000004</v>
+        <v>90.2667</v>
       </c>
       <c r="F98">
         <v>783369</v>
@@ -4139,10 +4121,10 @@
         <v>406</v>
       </c>
       <c r="D99">
-        <v>26.483339999999998</v>
+        <v>26.491557</v>
       </c>
       <c r="E99">
-        <v>89.634680000000003</v>
+        <v>89.592398000000003</v>
       </c>
       <c r="F99">
         <v>736208</v>
@@ -4159,10 +4141,10 @@
         <v>407</v>
       </c>
       <c r="D100">
-        <v>26.33</v>
+        <v>26.335833300000001</v>
       </c>
       <c r="E100">
-        <v>90.13</v>
+        <v>90.111194400000002</v>
       </c>
       <c r="F100">
         <v>783337</v>
@@ -4179,10 +4161,10 @@
         <v>408</v>
       </c>
       <c r="D101">
-        <v>26.427299999999999</v>
+        <v>26.403694399999999</v>
       </c>
       <c r="E101">
-        <v>89.905299999999997</v>
+        <v>90.272194400000004</v>
       </c>
       <c r="F101">
         <v>783333</v>
@@ -4199,10 +4181,10 @@
         <v>409</v>
       </c>
       <c r="D102">
-        <v>26.885850000000001</v>
+        <v>26.70025</v>
       </c>
       <c r="E102">
-        <v>88.474090000000004</v>
+        <v>88.413611099999997</v>
       </c>
       <c r="F102">
         <v>734005</v>
@@ -4219,10 +4201,10 @@
         <v>410</v>
       </c>
       <c r="D103">
-        <v>26.582550999999999</v>
+        <v>26.59</v>
       </c>
       <c r="E103">
-        <v>89.004932999999994</v>
+        <v>89.01</v>
       </c>
       <c r="F103">
         <v>735210</v>
@@ -4239,10 +4221,10 @@
         <v>411</v>
       </c>
       <c r="D104">
-        <v>26.1189</v>
+        <v>26.127479999999998</v>
       </c>
       <c r="E104">
-        <v>90.025599999999997</v>
+        <v>90.027100000000004</v>
       </c>
       <c r="F104">
         <v>783339</v>
@@ -4259,10 +4241,10 @@
         <v>412</v>
       </c>
       <c r="D105">
-        <v>26.357099999999999</v>
+        <v>26.3369167</v>
       </c>
       <c r="E105">
-        <v>90.641999999999996</v>
+        <v>90.664083300000001</v>
       </c>
       <c r="F105">
         <v>783384</v>
@@ -4279,10 +4261,10 @@
         <v>413</v>
       </c>
       <c r="D106">
-        <v>26.1021</v>
+        <v>26.114529999999998</v>
       </c>
       <c r="E106">
-        <v>91.616600000000005</v>
+        <v>91.612930000000006</v>
       </c>
       <c r="F106">
         <v>781017</v>
@@ -4299,10 +4281,10 @@
         <v>414</v>
       </c>
       <c r="D107">
-        <v>27.010541100000001</v>
+        <v>27.292853999999998</v>
       </c>
       <c r="E107">
-        <v>92.646216199999998</v>
+        <v>92.497433999999998</v>
       </c>
       <c r="F107">
         <v>790114</v>
@@ -4319,10 +4301,10 @@
         <v>415</v>
       </c>
       <c r="D108">
-        <v>26.341799999999999</v>
+        <v>26.345683999999999</v>
       </c>
       <c r="E108">
-        <v>91.689400000000006</v>
+        <v>91.689828000000006</v>
       </c>
       <c r="F108">
         <v>781380</v>
@@ -4339,10 +4321,10 @@
         <v>416</v>
       </c>
       <c r="D109">
-        <v>26.496766000000001</v>
+        <v>26.496972199999998</v>
       </c>
       <c r="E109">
-        <v>90.701598200000006</v>
+        <v>90.703666699999999</v>
       </c>
       <c r="F109">
         <v>783390</v>
@@ -4359,10 +4341,10 @@
         <v>417</v>
       </c>
       <c r="D110">
-        <v>26.708500000000001</v>
+        <v>26.7455</v>
       </c>
       <c r="E110">
-        <v>92.734300000000005</v>
+        <v>92.737499999999997</v>
       </c>
       <c r="F110">
         <v>784502</v>
@@ -4379,10 +4361,10 @@
         <v>418</v>
       </c>
       <c r="D111">
-        <v>25.991614999999999</v>
+        <v>26.1887778</v>
       </c>
       <c r="E111">
-        <v>91.257819999999995</v>
+        <v>91.745638900000003</v>
       </c>
       <c r="F111">
         <v>781141</v>
@@ -4399,10 +4381,10 @@
         <v>419</v>
       </c>
       <c r="D112">
-        <v>26.4786</v>
+        <v>26.481166699999999</v>
       </c>
       <c r="E112">
-        <v>90.560100000000006</v>
+        <v>90.521305600000005</v>
       </c>
       <c r="F112">
         <v>783381</v>
@@ -4419,10 +4401,10 @@
         <v>420</v>
       </c>
       <c r="D113">
-        <v>25.999600000000001</v>
+        <v>25.9734722</v>
       </c>
       <c r="E113">
-        <v>91.218900000000005</v>
+        <v>91.229027799999997</v>
       </c>
       <c r="F113">
         <v>781123</v>
@@ -4439,10 +4421,10 @@
         <v>421</v>
       </c>
       <c r="D114">
-        <v>26.502300000000002</v>
+        <v>26.3291389</v>
       </c>
       <c r="E114">
-        <v>90.964100000000002</v>
+        <v>91.010249999999999</v>
       </c>
       <c r="F114">
         <v>781315</v>
@@ -4459,10 +4441,10 @@
         <v>422</v>
       </c>
       <c r="D115">
-        <v>26.822530499999999</v>
+        <v>26.827349999999999</v>
       </c>
       <c r="E115">
-        <v>92.779871799999995</v>
+        <v>92.783450000000002</v>
       </c>
       <c r="F115">
         <v>784101</v>
@@ -4479,10 +4461,10 @@
         <v>423</v>
       </c>
       <c r="D116">
-        <v>26.2637693</v>
+        <v>26.2628333</v>
       </c>
       <c r="E116">
-        <v>91.693028699999999</v>
+        <v>91.695944400000002</v>
       </c>
       <c r="F116">
         <v>781101</v>
@@ -4499,10 +4481,10 @@
         <v>424</v>
       </c>
       <c r="D117">
-        <v>26.4925</v>
+        <v>26.275600000000001</v>
       </c>
       <c r="E117">
-        <v>90.612200000000001</v>
+        <v>90.334000000000003</v>
       </c>
       <c r="F117">
         <v>783380</v>
@@ -4519,10 +4501,10 @@
         <v>425</v>
       </c>
       <c r="D118">
-        <v>26.0015</v>
+        <v>25.542899999999999</v>
       </c>
       <c r="E118">
-        <v>90.761899999999997</v>
+        <v>90.462599999999995</v>
       </c>
       <c r="F118">
         <v>783124</v>
@@ -4539,10 +4521,10 @@
         <v>426</v>
       </c>
       <c r="D119">
-        <v>26.809799999999999</v>
+        <v>26.620827999999999</v>
       </c>
       <c r="E119">
-        <v>92.451599999999999</v>
+        <v>92.799014</v>
       </c>
       <c r="F119">
         <v>784110</v>
@@ -4559,10 +4541,10 @@
         <v>427</v>
       </c>
       <c r="D120">
-        <v>26.791399999999999</v>
+        <v>26.87987</v>
       </c>
       <c r="E120">
-        <v>92.923199999999994</v>
+        <v>93.052099999999996</v>
       </c>
       <c r="F120">
         <v>784182</v>
@@ -4579,10 +4561,10 @@
         <v>428</v>
       </c>
       <c r="D121">
-        <v>26.469291900000002</v>
+        <v>26.481166699999999</v>
       </c>
       <c r="E121">
-        <v>90.495125400000006</v>
+        <v>90.521305600000005</v>
       </c>
       <c r="F121">
         <v>783381</v>
@@ -4599,10 +4581,10 @@
         <v>429</v>
       </c>
       <c r="D122">
-        <v>26.517486999999999</v>
+        <v>26.52</v>
       </c>
       <c r="E122">
-        <v>89.203918000000002</v>
+        <v>89.2</v>
       </c>
       <c r="F122">
         <v>735211</v>
@@ -4618,12 +4600,6 @@
       <c r="C123" t="s">
         <v>430</v>
       </c>
-      <c r="D123">
-        <v>26.17</v>
-      </c>
-      <c r="E123">
-        <v>90.620002999999997</v>
-      </c>
       <c r="F123">
         <v>783121</v>
       </c>
@@ -4639,10 +4615,10 @@
         <v>431</v>
       </c>
       <c r="D124">
-        <v>27.1368531</v>
+        <v>27.145250000000001</v>
       </c>
       <c r="E124">
-        <v>93.791520000000006</v>
+        <v>93.752111110000001</v>
       </c>
       <c r="F124">
         <v>791112</v>
@@ -4659,10 +4635,10 @@
         <v>432</v>
       </c>
       <c r="D125">
-        <v>26.635349999999999</v>
+        <v>26.270700000000001</v>
       </c>
       <c r="E125">
-        <v>91.243880000000004</v>
+        <v>91.313500000000005</v>
       </c>
       <c r="F125">
         <v>781369</v>
@@ -4679,10 +4655,10 @@
         <v>433</v>
       </c>
       <c r="D126">
-        <v>26.5274</v>
+        <v>26.315899999999999</v>
       </c>
       <c r="E126">
-        <v>91.721500000000006</v>
+        <v>91.4345</v>
       </c>
       <c r="F126">
         <v>781366</v>
@@ -4699,10 +4675,10 @@
         <v>434</v>
       </c>
       <c r="D127">
-        <v>26.851208499999998</v>
+        <v>26.654250000000001</v>
       </c>
       <c r="E127">
-        <v>93.461073799999994</v>
+        <v>92.801150000000007</v>
       </c>
       <c r="F127">
         <v>784170</v>
@@ -4719,10 +4695,10 @@
         <v>435</v>
       </c>
       <c r="D128">
-        <v>27.1191</v>
+        <v>27.119472200000001</v>
       </c>
       <c r="E128">
-        <v>93.860600000000005</v>
+        <v>93.930388899999997</v>
       </c>
       <c r="F128">
         <v>784160</v>
@@ -4739,10 +4715,10 @@
         <v>436</v>
       </c>
       <c r="D129">
-        <v>26.688800000000001</v>
+        <v>26.6866181</v>
       </c>
       <c r="E129">
-        <v>89.421000000000006</v>
+        <v>89.429294499999997</v>
       </c>
       <c r="F129">
         <v>735214</v>
@@ -4759,10 +4735,10 @@
         <v>437</v>
       </c>
       <c r="D130">
-        <v>26.7210185</v>
+        <v>26.7003433</v>
       </c>
       <c r="E130">
-        <v>91.990599599999996</v>
+        <v>91.949126199999995</v>
       </c>
       <c r="F130">
         <v>784510</v>
@@ -4779,10 +4755,10 @@
         <v>438</v>
       </c>
       <c r="D131">
-        <v>26.240379999999998</v>
+        <v>26.135400000000001</v>
       </c>
       <c r="E131">
-        <v>90.575460000000007</v>
+        <v>90.341300000000004</v>
       </c>
       <c r="F131">
         <v>783382</v>
@@ -4799,10 +4775,10 @@
         <v>439</v>
       </c>
       <c r="D132">
-        <v>26.6025201</v>
+        <v>26.617958699999999</v>
       </c>
       <c r="E132">
-        <v>91.817206900000002</v>
+        <v>91.817885399999994</v>
       </c>
       <c r="F132">
         <v>784522</v>
@@ -4819,10 +4795,10 @@
         <v>440</v>
       </c>
       <c r="D133">
-        <v>26.115103000000001</v>
+        <v>26.345683999999999</v>
       </c>
       <c r="E133">
-        <v>91.703238999999996</v>
+        <v>91.689828000000006</v>
       </c>
       <c r="F133">
         <v>781380</v>
@@ -4839,10 +4815,10 @@
         <v>441</v>
       </c>
       <c r="D134">
-        <v>26.070699999999999</v>
+        <v>26.0276</v>
       </c>
       <c r="E134">
-        <v>90.682299999999998</v>
+        <v>90.500200000000007</v>
       </c>
       <c r="F134">
         <v>783126</v>
@@ -4859,10 +4835,10 @@
         <v>442</v>
       </c>
       <c r="D135">
-        <v>26.450734799999999</v>
+        <v>26.270099999999999</v>
       </c>
       <c r="E135">
-        <v>91.336927399999993</v>
+        <v>91.201999999999998</v>
       </c>
       <c r="F135">
         <v>781370</v>
@@ -4879,10 +4855,10 @@
         <v>443</v>
       </c>
       <c r="D136">
-        <v>27.199539999999999</v>
+        <v>27.2311944</v>
       </c>
       <c r="E136">
-        <v>94.099069999999998</v>
+        <v>94.092194399999997</v>
       </c>
       <c r="F136">
         <v>787031</v>
@@ -4899,10 +4875,10 @@
         <v>444</v>
       </c>
       <c r="D137">
-        <v>26.463321000000001</v>
+        <v>26.1887778</v>
       </c>
       <c r="E137">
-        <v>91.642769000000001</v>
+        <v>91.745638900000003</v>
       </c>
       <c r="F137">
         <v>781354</v>
@@ -4919,10 +4895,10 @@
         <v>445</v>
       </c>
       <c r="D138">
-        <v>26.073</v>
+        <v>26.088027799999999</v>
       </c>
       <c r="E138">
-        <v>91.518000000000001</v>
+        <v>91.535555599999995</v>
       </c>
       <c r="F138">
         <v>781125</v>
@@ -4939,10 +4915,10 @@
         <v>446</v>
       </c>
       <c r="D139">
-        <v>26.376031999999999</v>
+        <v>26.481166699999999</v>
       </c>
       <c r="E139">
-        <v>91.770920000000004</v>
+        <v>90.521305600000005</v>
       </c>
       <c r="F139">
         <v>783381</v>
@@ -4959,10 +4935,10 @@
         <v>447</v>
       </c>
       <c r="D140">
-        <v>26.67248</v>
+        <v>26.7362289</v>
       </c>
       <c r="E140">
-        <v>92.8964</v>
+        <v>93.046352799999994</v>
       </c>
       <c r="F140">
         <v>784175</v>
@@ -4979,10 +4955,10 @@
         <v>448</v>
       </c>
       <c r="D141">
-        <v>27.130800000000001</v>
+        <v>27.105833329999999</v>
       </c>
       <c r="E141">
-        <v>93.709500000000006</v>
+        <v>93.693083329999993</v>
       </c>
       <c r="F141">
         <v>791110</v>
@@ -4999,10 +4975,10 @@
         <v>449</v>
       </c>
       <c r="D142">
-        <v>26.450900000000001</v>
+        <v>26.444777800000001</v>
       </c>
       <c r="E142">
-        <v>91.439700000000002</v>
+        <v>91.438000000000002</v>
       </c>
       <c r="F142">
         <v>781335</v>
@@ -5019,10 +4995,10 @@
         <v>450</v>
       </c>
       <c r="D143">
-        <v>26.8109</v>
+        <v>26.816017899999999</v>
       </c>
       <c r="E143">
-        <v>92.577349999999996</v>
+        <v>92.582411100000002</v>
       </c>
       <c r="F143">
         <v>784506</v>
@@ -5039,10 +5015,10 @@
         <v>451</v>
       </c>
       <c r="D144">
-        <v>26.499382000000001</v>
+        <v>26.300999999999998</v>
       </c>
       <c r="E144">
-        <v>91.179271</v>
+        <v>91.104200000000006</v>
       </c>
       <c r="F144">
         <v>781325</v>
@@ -5059,10 +5035,10 @@
         <v>452</v>
       </c>
       <c r="D145">
-        <v>26.115103000000001</v>
+        <v>26.161305599999999</v>
       </c>
       <c r="E145">
-        <v>91.703238999999996</v>
+        <v>90.621611099999996</v>
       </c>
       <c r="F145">
         <v>783101</v>
@@ -5079,10 +5055,10 @@
         <v>453</v>
       </c>
       <c r="D146">
-        <v>26.502672100000002</v>
+        <v>26.272600000000001</v>
       </c>
       <c r="E146">
-        <v>90.807977199999996</v>
+        <v>90.345200000000006</v>
       </c>
       <c r="F146">
         <v>783391</v>
@@ -5099,10 +5075,10 @@
         <v>454</v>
       </c>
       <c r="D147">
-        <v>26.446899999999999</v>
+        <v>26.441690000000001</v>
       </c>
       <c r="E147">
-        <v>91.606499999999997</v>
+        <v>91.610420000000005</v>
       </c>
       <c r="F147">
         <v>781365</v>
@@ -5119,10 +5095,10 @@
         <v>455</v>
       </c>
       <c r="D148">
-        <v>26.8218</v>
+        <v>26.821432399999999</v>
       </c>
       <c r="E148">
-        <v>92.683099999999996</v>
+        <v>92.682479000000001</v>
       </c>
       <c r="F148">
         <v>784505</v>
@@ -5139,10 +5115,10 @@
         <v>456</v>
       </c>
       <c r="D149">
-        <v>26.737349999999999</v>
+        <v>26.746832900000001</v>
       </c>
       <c r="E149">
-        <v>92.215180000000004</v>
+        <v>92.151521299999999</v>
       </c>
       <c r="F149">
         <v>784508</v>
@@ -5159,10 +5135,10 @@
         <v>457</v>
       </c>
       <c r="D150">
-        <v>26.4938842</v>
+        <v>26.491972199999999</v>
       </c>
       <c r="E150">
-        <v>90.884529099999995</v>
+        <v>90.886194399999994</v>
       </c>
       <c r="F150">
         <v>781317</v>
@@ -5179,10 +5155,10 @@
         <v>458</v>
       </c>
       <c r="D151">
-        <v>27.200871500000002</v>
+        <v>27.2311944</v>
       </c>
       <c r="E151">
-        <v>94.031376199999997</v>
+        <v>94.092194399999997</v>
       </c>
       <c r="F151">
         <v>787031</v>
@@ -5199,10 +5175,10 @@
         <v>459</v>
       </c>
       <c r="D152">
-        <v>26.4995203</v>
+        <v>26.285599999999999</v>
       </c>
       <c r="E152">
-        <v>91.077335199999993</v>
+        <v>90.574200000000005</v>
       </c>
       <c r="F152">
         <v>781313</v>
@@ -5218,12 +5194,6 @@
       <c r="C153" t="s">
         <v>460</v>
       </c>
-      <c r="D153">
-        <v>26.980030200000002</v>
-      </c>
-      <c r="E153">
-        <v>93.819766000000001</v>
-      </c>
       <c r="F153">
         <v>786164</v>
       </c>
@@ -5239,10 +5209,10 @@
         <v>461</v>
       </c>
       <c r="D154">
-        <v>26.471299999999999</v>
+        <v>26.4748889</v>
       </c>
       <c r="E154">
-        <v>91.267799999999994</v>
+        <v>91.269083300000005</v>
       </c>
       <c r="F154">
         <v>781371</v>
@@ -5259,10 +5229,10 @@
         <v>462</v>
       </c>
       <c r="D155">
-        <v>26.75703</v>
+        <v>26.663198999999999</v>
       </c>
       <c r="E155">
-        <v>91.943719999999999</v>
+        <v>91.920809700000007</v>
       </c>
       <c r="F155">
         <v>784521</v>
@@ -5279,10 +5249,10 @@
         <v>463</v>
       </c>
       <c r="D156">
-        <v>28.188173200000001</v>
+        <v>27.2836389</v>
       </c>
       <c r="E156">
-        <v>85.121445199999997</v>
+        <v>95.333527799999999</v>
       </c>
       <c r="F156">
         <v>786610</v>
@@ -5299,10 +5269,10 @@
         <v>464</v>
       </c>
       <c r="D157">
-        <v>26.744599999999998</v>
+        <v>26.735220099999999</v>
       </c>
       <c r="E157">
-        <v>92.097099999999998</v>
+        <v>92.105292700000007</v>
       </c>
       <c r="F157">
         <v>784509</v>
@@ -5319,10 +5289,10 @@
         <v>465</v>
       </c>
       <c r="D158">
-        <v>26.73732</v>
+        <v>26.710899999999999</v>
       </c>
       <c r="E158">
-        <v>93.198053000000002</v>
+        <v>93.172250000000005</v>
       </c>
       <c r="F158">
         <v>784176</v>
@@ -5339,10 +5309,10 @@
         <v>466</v>
       </c>
       <c r="D159">
-        <v>23.924769999999999</v>
+        <v>23.921722219999999</v>
       </c>
       <c r="E159">
-        <v>91.846466000000007</v>
+        <v>91.850611110000003</v>
       </c>
       <c r="F159">
         <v>799289</v>
@@ -5359,10 +5329,10 @@
         <v>467</v>
       </c>
       <c r="D160">
-        <v>26.200888899999999</v>
+        <v>26.183472200000001</v>
       </c>
       <c r="E160">
-        <v>91.686011100000002</v>
+        <v>91.696166700000006</v>
       </c>
       <c r="F160">
         <v>781031</v>
@@ -5379,10 +5349,10 @@
         <v>468</v>
       </c>
       <c r="D161">
-        <v>23.792899999999999</v>
+        <v>23.81177778</v>
       </c>
       <c r="E161">
-        <v>91.278400000000005</v>
+        <v>91.267666669999997</v>
       </c>
       <c r="F161">
         <v>799003</v>
@@ -5399,10 +5369,10 @@
         <v>469</v>
       </c>
       <c r="D162">
-        <v>26.595420000000001</v>
+        <v>26.350300000000001</v>
       </c>
       <c r="E162">
-        <v>92.326220000000006</v>
+        <v>92.6922</v>
       </c>
       <c r="F162">
         <v>782411</v>
@@ -5419,10 +5389,10 @@
         <v>470</v>
       </c>
       <c r="D163">
-        <v>26.354389999999999</v>
+        <v>26.281300000000002</v>
       </c>
       <c r="E163">
-        <v>93.926119999999997</v>
+        <v>93.884</v>
       </c>
       <c r="F163">
         <v>785602</v>
@@ -5439,10 +5409,10 @@
         <v>471</v>
       </c>
       <c r="D164">
-        <v>23.673954200000001</v>
+        <v>23.674027779999999</v>
       </c>
       <c r="E164">
-        <v>91.2816811</v>
+        <v>91.282250000000005</v>
       </c>
       <c r="F164">
         <v>799102</v>
@@ -5459,10 +5429,10 @@
         <v>472</v>
       </c>
       <c r="D165">
-        <v>24.865100000000002</v>
+        <v>24.867584000000001</v>
       </c>
       <c r="E165">
-        <v>92.555800000000005</v>
+        <v>92.360382000000001</v>
       </c>
       <c r="F165">
         <v>788806</v>
@@ -5479,10 +5449,10 @@
         <v>473</v>
       </c>
       <c r="D166">
-        <v>24.6829</v>
+        <v>24.68</v>
       </c>
       <c r="E166">
-        <v>92.341200000000001</v>
+        <v>92.34</v>
       </c>
       <c r="F166">
         <v>788723</v>
@@ -5499,10 +5469,10 @@
         <v>474</v>
       </c>
       <c r="D167">
-        <v>26.116303800000001</v>
+        <v>26.1887778</v>
       </c>
       <c r="E167">
-        <v>92.139522999999997</v>
+        <v>91.745638900000003</v>
       </c>
       <c r="F167">
         <v>782403</v>
@@ -5519,10 +5489,10 @@
         <v>475</v>
       </c>
       <c r="D168">
-        <v>25.755099999999999</v>
+        <v>25.839444400000001</v>
       </c>
       <c r="E168">
-        <v>93.243099999999998</v>
+        <v>93.437694399999998</v>
       </c>
       <c r="F168">
         <v>782460</v>
@@ -5539,10 +5509,10 @@
         <v>476</v>
       </c>
       <c r="D169">
-        <v>26.019400000000001</v>
+        <v>26.0242778</v>
       </c>
       <c r="E169">
-        <v>93.780199999999994</v>
+        <v>93.772055600000002</v>
       </c>
       <c r="F169">
         <v>782480</v>
@@ -5559,10 +5529,10 @@
         <v>477</v>
       </c>
       <c r="D170">
-        <v>26.2957</v>
+        <v>26.281300000000002</v>
       </c>
       <c r="E170">
-        <v>93.860500000000002</v>
+        <v>93.884</v>
       </c>
       <c r="F170">
         <v>785602</v>
@@ -5579,10 +5549,10 @@
         <v>478</v>
       </c>
       <c r="D171">
-        <v>24.36927</v>
+        <v>24.437103</v>
       </c>
       <c r="E171">
-        <v>92.205250000000007</v>
+        <v>92.242231000000004</v>
       </c>
       <c r="F171">
         <v>799262</v>
@@ -5599,10 +5569,10 @@
         <v>479</v>
       </c>
       <c r="D172">
-        <v>26.359349999999999</v>
+        <v>26.197833299999999</v>
       </c>
       <c r="E172">
-        <v>94.062659999999994</v>
+        <v>93.8606944</v>
       </c>
       <c r="F172">
         <v>785601</v>
@@ -5619,10 +5589,10 @@
         <v>480</v>
       </c>
       <c r="D173">
-        <v>25.046292999999999</v>
+        <v>24.44</v>
       </c>
       <c r="E173">
-        <v>92.678509000000005</v>
+        <v>92.29</v>
       </c>
       <c r="F173">
         <v>788817</v>
@@ -5639,10 +5609,10 @@
         <v>481</v>
       </c>
       <c r="D174">
-        <v>25.039300000000001</v>
+        <v>26.121400000000001</v>
       </c>
       <c r="E174">
-        <v>88.119510000000005</v>
+        <v>92.305700000000002</v>
       </c>
       <c r="F174">
         <v>782425</v>
@@ -5659,10 +5629,10 @@
         <v>482</v>
       </c>
       <c r="D175">
-        <v>24.248670000000001</v>
+        <v>24.1417</v>
       </c>
       <c r="E175">
-        <v>92.200239999999994</v>
+        <v>92.173199999999994</v>
       </c>
       <c r="F175">
         <v>799256</v>
@@ -5679,10 +5649,10 @@
         <v>483</v>
       </c>
       <c r="D176">
-        <v>26.157330999999999</v>
+        <v>26.1401</v>
       </c>
       <c r="E176">
-        <v>92.017523999999995</v>
+        <v>91.5625</v>
       </c>
       <c r="F176">
         <v>782401</v>
@@ -5699,10 +5669,10 @@
         <v>484</v>
       </c>
       <c r="D177">
-        <v>26.931450000000002</v>
+        <v>26.9886944</v>
       </c>
       <c r="E177">
-        <v>94.747699999999995</v>
+        <v>94.631888900000007</v>
       </c>
       <c r="F177">
         <v>785685</v>
@@ -5719,10 +5689,10 @@
         <v>485</v>
       </c>
       <c r="D178">
-        <v>25.158750000000001</v>
+        <v>24.823637000000002</v>
       </c>
       <c r="E178">
-        <v>93.104330000000004</v>
+        <v>92.801827000000003</v>
       </c>
       <c r="F178">
         <v>788830</v>
@@ -5779,10 +5749,10 @@
         <v>488</v>
       </c>
       <c r="D181">
-        <v>25.80462</v>
+        <v>25.90583333</v>
       </c>
       <c r="E181">
-        <v>93.750100000000003</v>
+        <v>93.739333329999994</v>
       </c>
       <c r="F181">
         <v>797112</v>
@@ -5799,10 +5769,10 @@
         <v>489</v>
       </c>
       <c r="D182">
-        <v>25.906669999999998</v>
+        <v>25.839444400000001</v>
       </c>
       <c r="E182">
-        <v>93.439279999999997</v>
+        <v>93.437694399999998</v>
       </c>
       <c r="F182">
         <v>782460</v>
@@ -5819,10 +5789,10 @@
         <v>490</v>
       </c>
       <c r="D183">
-        <v>26.02101</v>
+        <v>26.0242778</v>
       </c>
       <c r="E183">
-        <v>93.764319999999998</v>
+        <v>93.772055600000002</v>
       </c>
       <c r="F183">
         <v>782480</v>
@@ -5839,10 +5809,10 @@
         <v>491</v>
       </c>
       <c r="D184">
-        <v>26.187169999999998</v>
+        <v>26.1887778</v>
       </c>
       <c r="E184">
-        <v>91.743340000000003</v>
+        <v>91.745638900000003</v>
       </c>
       <c r="F184">
         <v>781001</v>
@@ -5859,10 +5829,10 @@
         <v>492</v>
       </c>
       <c r="D185">
-        <v>26.341090000000001</v>
+        <v>26.351749999999999</v>
       </c>
       <c r="E185">
-        <v>92.664739999999995</v>
+        <v>92.678277800000004</v>
       </c>
       <c r="F185">
         <v>782002</v>
@@ -5879,10 +5849,10 @@
         <v>493</v>
       </c>
       <c r="D186">
-        <v>26.002050000000001</v>
+        <v>26.348694399999999</v>
       </c>
       <c r="E186">
-        <v>92.827796000000006</v>
+        <v>92.700500000000005</v>
       </c>
       <c r="F186">
         <v>782435</v>
@@ -5899,10 +5869,10 @@
         <v>494</v>
       </c>
       <c r="D187">
-        <v>25.105920000000001</v>
+        <v>24.823637000000002</v>
       </c>
       <c r="E187">
-        <v>92.895920000000004</v>
+        <v>92.801827000000003</v>
       </c>
       <c r="F187">
         <v>788818</v>
@@ -5919,10 +5889,10 @@
         <v>495</v>
       </c>
       <c r="D188">
-        <v>25.754159999999999</v>
+        <v>26.348694399999999</v>
       </c>
       <c r="E188">
-        <v>93.264420000000001</v>
+        <v>92.700500000000005</v>
       </c>
       <c r="F188">
         <v>782446</v>
@@ -5939,10 +5909,10 @@
         <v>496</v>
       </c>
       <c r="D189">
-        <v>25.039300000000001</v>
+        <v>26.350300000000001</v>
       </c>
       <c r="E189">
-        <v>88.119510000000005</v>
+        <v>92.6922</v>
       </c>
       <c r="F189">
         <v>782429</v>
@@ -5959,10 +5929,10 @@
         <v>497</v>
       </c>
       <c r="D190">
-        <v>23.81634</v>
+        <v>23.824472220000001</v>
       </c>
       <c r="E190">
-        <v>91.280540000000002</v>
+        <v>91.29216667</v>
       </c>
       <c r="F190">
         <v>799004</v>
@@ -5979,10 +5949,10 @@
         <v>498</v>
       </c>
       <c r="D191">
-        <v>25.95316</v>
+        <v>26.123750000000001</v>
       </c>
       <c r="E191">
-        <v>92.243348999999995</v>
+        <v>92.198583299999996</v>
       </c>
       <c r="F191">
         <v>782410</v>
@@ -5999,10 +5969,10 @@
         <v>499</v>
       </c>
       <c r="D192">
-        <v>26.339945</v>
+        <v>26.1114</v>
       </c>
       <c r="E192">
-        <v>94.008256000000003</v>
+        <v>92.142600000000002</v>
       </c>
       <c r="F192">
         <v>785603</v>
@@ -6019,10 +5989,10 @@
         <v>500</v>
       </c>
       <c r="D193">
-        <v>26.009620000000002</v>
+        <v>26.1069</v>
       </c>
       <c r="E193">
-        <v>92.831789999999998</v>
+        <v>92.745599999999996</v>
       </c>
       <c r="F193">
         <v>782428</v>
@@ -6039,10 +6009,10 @@
         <v>501</v>
       </c>
       <c r="D194">
-        <v>23.852709999999998</v>
+        <v>23.832823000000001</v>
       </c>
       <c r="E194">
-        <v>91.287779999999998</v>
+        <v>91.368358000000001</v>
       </c>
       <c r="F194">
         <v>799035</v>
@@ -6059,10 +6029,10 @@
         <v>502</v>
       </c>
       <c r="D195">
-        <v>25.105920000000001</v>
+        <v>24.823637000000002</v>
       </c>
       <c r="E195">
-        <v>92.895920000000004</v>
+        <v>92.801827000000003</v>
       </c>
       <c r="F195">
         <v>788818</v>
@@ -6079,10 +6049,10 @@
         <v>503</v>
       </c>
       <c r="D196">
-        <v>26.02101</v>
+        <v>26.0242778</v>
       </c>
       <c r="E196">
-        <v>93.764319999999998</v>
+        <v>93.772055600000002</v>
       </c>
       <c r="F196">
         <v>782480</v>
@@ -6099,10 +6069,10 @@
         <v>504</v>
       </c>
       <c r="D197">
-        <v>26.250039999999998</v>
+        <v>26.1887778</v>
       </c>
       <c r="E197">
-        <v>91.556820000000002</v>
+        <v>91.745638900000003</v>
       </c>
       <c r="F197">
         <v>782403</v>
@@ -6119,10 +6089,10 @@
         <v>505</v>
       </c>
       <c r="D198">
-        <v>24.113040000000002</v>
+        <v>24.162388889999999</v>
       </c>
       <c r="E198">
-        <v>92.022859999999994</v>
+        <v>92.03797222</v>
       </c>
       <c r="F198">
         <v>799264</v>
@@ -6139,10 +6109,10 @@
         <v>506</v>
       </c>
       <c r="D199">
-        <v>24.603216</v>
+        <v>24.823637000000002</v>
       </c>
       <c r="E199">
-        <v>92.907608999999994</v>
+        <v>92.801827000000003</v>
       </c>
       <c r="F199">
         <v>788116</v>
@@ -6159,10 +6129,10 @@
         <v>507</v>
       </c>
       <c r="D200">
-        <v>24.113040000000002</v>
+        <v>24.162388889999999</v>
       </c>
       <c r="E200">
-        <v>92.022859999999994</v>
+        <v>92.03797222</v>
       </c>
       <c r="F200">
         <v>799264</v>
@@ -6179,10 +6149,10 @@
         <v>508</v>
       </c>
       <c r="D201">
-        <v>26.040317999999999</v>
+        <v>26.157861100000002</v>
       </c>
       <c r="E201">
-        <v>92.678509000000005</v>
+        <v>92.659277799999998</v>
       </c>
       <c r="F201">
         <v>782426</v>
@@ -6199,10 +6169,10 @@
         <v>509</v>
       </c>
       <c r="D202">
-        <v>22.491109999999999</v>
+        <v>24.867584000000001</v>
       </c>
       <c r="E202">
-        <v>88.316410000000005</v>
+        <v>92.360382000000001</v>
       </c>
       <c r="F202">
         <v>788710</v>
@@ -6219,10 +6189,10 @@
         <v>510</v>
       </c>
       <c r="D203">
-        <v>26.164328999999999</v>
+        <v>26.160620000000002</v>
       </c>
       <c r="E203">
-        <v>91.702802000000005</v>
+        <v>91.709479999999999</v>
       </c>
       <c r="F203">
         <v>781010</v>
@@ -6239,10 +6209,10 @@
         <v>511</v>
       </c>
       <c r="D204">
-        <v>25.754159999999999</v>
+        <v>26.348694399999999</v>
       </c>
       <c r="E204">
-        <v>93.264420000000001</v>
+        <v>92.700500000000005</v>
       </c>
       <c r="F204">
         <v>782447</v>
@@ -6259,10 +6229,10 @@
         <v>512</v>
       </c>
       <c r="D205">
-        <v>25.168289999999999</v>
+        <v>24.823637000000002</v>
       </c>
       <c r="E205">
-        <v>93.009569999999997</v>
+        <v>92.801827000000003</v>
       </c>
       <c r="F205">
         <v>788819</v>
@@ -6279,10 +6249,10 @@
         <v>513</v>
       </c>
       <c r="D206">
-        <v>24.453710000000001</v>
+        <v>26.350300000000001</v>
       </c>
       <c r="E206">
-        <v>74.861429999999999</v>
+        <v>92.6922</v>
       </c>
       <c r="F206">
         <v>782442</v>
@@ -6299,10 +6269,10 @@
         <v>514</v>
       </c>
       <c r="D207">
-        <v>25.754159999999999</v>
+        <v>26.348694399999999</v>
       </c>
       <c r="E207">
-        <v>93.264420000000001</v>
+        <v>92.700500000000005</v>
       </c>
       <c r="F207">
         <v>782446</v>
@@ -6319,10 +6289,10 @@
         <v>515</v>
       </c>
       <c r="D208">
-        <v>25.754159999999999</v>
+        <v>26.348694399999999</v>
       </c>
       <c r="E208">
-        <v>93.264420000000001</v>
+        <v>92.700500000000005</v>
       </c>
       <c r="F208">
         <v>782447</v>
@@ -6339,10 +6309,10 @@
         <v>516</v>
       </c>
       <c r="D209">
-        <v>25.754159999999999</v>
+        <v>26.348694399999999</v>
       </c>
       <c r="E209">
-        <v>93.264420000000001</v>
+        <v>92.700500000000005</v>
       </c>
       <c r="F209">
         <v>782447</v>
@@ -6359,10 +6329,10 @@
         <v>517</v>
       </c>
       <c r="D210">
-        <v>25.039300000000001</v>
+        <v>26.121400000000001</v>
       </c>
       <c r="E210">
-        <v>88.119510000000005</v>
+        <v>92.305700000000002</v>
       </c>
       <c r="F210">
         <v>782425</v>
@@ -6399,10 +6369,10 @@
         <v>518</v>
       </c>
       <c r="D212">
-        <v>25.158750000000001</v>
+        <v>24.823637000000002</v>
       </c>
       <c r="E212">
-        <v>93.104330000000004</v>
+        <v>92.801827000000003</v>
       </c>
       <c r="F212">
         <v>788831</v>
@@ -6419,10 +6389,10 @@
         <v>519</v>
       </c>
       <c r="D213">
-        <v>23.665900000000001</v>
+        <v>23.840138889999999</v>
       </c>
       <c r="E213">
-        <v>91.71996</v>
+        <v>91.634611109999994</v>
       </c>
       <c r="F213">
         <v>799205</v>
@@ -6439,10 +6409,10 @@
         <v>520</v>
       </c>
       <c r="D214">
-        <v>25.716629999999999</v>
+        <v>24.823637000000002</v>
       </c>
       <c r="E214">
-        <v>93.126800000000003</v>
+        <v>92.801827000000003</v>
       </c>
       <c r="F214">
         <v>788832</v>
@@ -6459,10 +6429,10 @@
         <v>521</v>
       </c>
       <c r="D215">
-        <v>26.18402</v>
+        <v>26.1844167</v>
       </c>
       <c r="E215">
-        <v>91.757909999999995</v>
+        <v>91.768916700000005</v>
       </c>
       <c r="F215">
         <v>781003</v>
@@ -6479,10 +6449,10 @@
         <v>522</v>
       </c>
       <c r="D216">
-        <v>26.359349999999999</v>
+        <v>26.197833299999999</v>
       </c>
       <c r="E216">
-        <v>94.062659999999994</v>
+        <v>93.8606944</v>
       </c>
       <c r="F216">
         <v>785601</v>
@@ -6499,10 +6469,10 @@
         <v>523</v>
       </c>
       <c r="D217">
-        <v>24.826360000000001</v>
+        <v>24.867584000000001</v>
       </c>
       <c r="E217">
-        <v>92.300150000000002</v>
+        <v>92.360382000000001</v>
       </c>
       <c r="F217">
         <v>788722</v>
@@ -6519,10 +6489,10 @@
         <v>524</v>
       </c>
       <c r="D218">
-        <v>24.302230000000002</v>
+        <v>24.3788333</v>
       </c>
       <c r="E218">
-        <v>92.164360000000002</v>
+        <v>92.159805599999999</v>
       </c>
       <c r="F218">
         <v>799263</v>
@@ -6539,10 +6509,10 @@
         <v>525</v>
       </c>
       <c r="D219">
-        <v>25.754159999999999</v>
+        <v>26.348694399999999</v>
       </c>
       <c r="E219">
-        <v>93.264420000000001</v>
+        <v>92.700500000000005</v>
       </c>
       <c r="F219">
         <v>782447</v>
@@ -6559,10 +6529,10 @@
         <v>526</v>
       </c>
       <c r="D220">
-        <v>26.159427000000001</v>
+        <v>26.180540000000001</v>
       </c>
       <c r="E220">
-        <v>91.861101000000005</v>
+        <v>91.825090000000003</v>
       </c>
       <c r="F220">
         <v>781026</v>
@@ -6579,10 +6549,10 @@
         <v>527</v>
       </c>
       <c r="D221">
-        <v>26.339945</v>
+        <v>26.1114</v>
       </c>
       <c r="E221">
-        <v>94.008256000000003</v>
+        <v>92.142600000000002</v>
       </c>
       <c r="F221">
         <v>785603</v>
@@ -6599,10 +6569,10 @@
         <v>528</v>
       </c>
       <c r="D222">
-        <v>24.302230000000002</v>
+        <v>24.3788333</v>
       </c>
       <c r="E222">
-        <v>92.164360000000002</v>
+        <v>92.159805599999999</v>
       </c>
       <c r="F222">
         <v>799263</v>
@@ -6619,10 +6589,10 @@
         <v>529</v>
       </c>
       <c r="D223">
-        <v>26.159427000000001</v>
+        <v>26.180540000000001</v>
       </c>
       <c r="E223">
-        <v>91.861101000000005</v>
+        <v>91.825090000000003</v>
       </c>
       <c r="F223">
         <v>781026</v>
@@ -6639,10 +6609,10 @@
         <v>530</v>
       </c>
       <c r="D224">
-        <v>29.839141999999999</v>
+        <v>29.824249999999999</v>
       </c>
       <c r="E224">
-        <v>79.166140999999996</v>
+        <v>79.209166699999997</v>
       </c>
       <c r="F224">
         <v>263661</v>
@@ -6659,10 +6629,10 @@
         <v>531</v>
       </c>
       <c r="D225">
-        <v>24.864000999999998</v>
+        <v>24.86</v>
       </c>
       <c r="E225">
-        <v>92.594123999999994</v>
+        <v>92.59</v>
       </c>
       <c r="F225">
         <v>788802</v>
@@ -6679,10 +6649,10 @@
         <v>532</v>
       </c>
       <c r="D226">
-        <v>24.616019999999999</v>
+        <v>24.867584000000001</v>
       </c>
       <c r="E226">
-        <v>92.358159999999998</v>
+        <v>92.360382000000001</v>
       </c>
       <c r="F226">
         <v>788724</v>
@@ -6699,10 +6669,10 @@
         <v>533</v>
       </c>
       <c r="D227">
-        <v>39.390897000000002</v>
+        <v>28.61</v>
       </c>
       <c r="E227">
-        <v>-99.066067000000004</v>
+        <v>80.08</v>
       </c>
       <c r="F227">
         <v>788801</v>
@@ -6719,10 +6689,10 @@
         <v>534</v>
       </c>
       <c r="D228">
-        <v>26.234870999999998</v>
+        <v>26.262779999999999</v>
       </c>
       <c r="E228">
-        <v>92.693416999999997</v>
+        <v>92.641779999999997</v>
       </c>
       <c r="F228">
         <v>782144</v>
@@ -6739,10 +6709,10 @@
         <v>535</v>
       </c>
       <c r="D229">
-        <v>24.821829999999999</v>
+        <v>24.823637000000002</v>
       </c>
       <c r="E229">
-        <v>92.804649999999995</v>
+        <v>92.801827000000003</v>
       </c>
       <c r="F229">
         <v>788001</v>
@@ -6759,10 +6729,10 @@
         <v>536</v>
       </c>
       <c r="D230">
-        <v>25.816579999999998</v>
+        <v>25.863216000000001</v>
       </c>
       <c r="E230">
-        <v>93.784319999999994</v>
+        <v>93.754315000000005</v>
       </c>
       <c r="F230">
         <v>797115</v>
@@ -6779,10 +6749,10 @@
         <v>536</v>
       </c>
       <c r="D231">
-        <v>25.816579999999998</v>
+        <v>25.863216000000001</v>
       </c>
       <c r="E231">
-        <v>93.784319999999994</v>
+        <v>93.754315000000005</v>
       </c>
       <c r="F231">
         <v>797115</v>
@@ -6799,10 +6769,10 @@
         <v>537</v>
       </c>
       <c r="D232">
-        <v>26.379860000000001</v>
+        <v>26.273</v>
       </c>
       <c r="E232">
-        <v>91.023120000000006</v>
+        <v>90.511300000000006</v>
       </c>
       <c r="F232">
         <v>781321</v>
@@ -6819,10 +6789,10 @@
         <v>538</v>
       </c>
       <c r="D233">
-        <v>25.061077000000001</v>
+        <v>24.867584000000001</v>
       </c>
       <c r="E233">
-        <v>92.509890999999996</v>
+        <v>92.360382000000001</v>
       </c>
       <c r="F233">
         <v>788804</v>
@@ -6839,10 +6809,10 @@
         <v>539</v>
       </c>
       <c r="D234">
-        <v>26.359349999999999</v>
+        <v>26.197833299999999</v>
       </c>
       <c r="E234">
-        <v>94.062659999999994</v>
+        <v>93.8606944</v>
       </c>
       <c r="F234">
         <v>785601</v>
@@ -6859,10 +6829,10 @@
         <v>540</v>
       </c>
       <c r="D235">
-        <v>26.143830000000001</v>
+        <v>26.190300000000001</v>
       </c>
       <c r="E235">
-        <v>92.389160000000004</v>
+        <v>92.373900000000006</v>
       </c>
       <c r="F235">
         <v>782412</v>
@@ -6879,10 +6849,10 @@
         <v>541</v>
       </c>
       <c r="D236">
-        <v>23.665900000000001</v>
+        <v>23.840138889999999</v>
       </c>
       <c r="E236">
-        <v>91.71996</v>
+        <v>91.634611109999994</v>
       </c>
       <c r="F236">
         <v>799205</v>
@@ -6899,10 +6869,10 @@
         <v>542</v>
       </c>
       <c r="D237">
-        <v>26.245024000000001</v>
+        <v>26.145499999999998</v>
       </c>
       <c r="E237">
-        <v>91.617801</v>
+        <v>91.341800000000006</v>
       </c>
       <c r="F237">
         <v>781104</v>
@@ -6919,10 +6889,10 @@
         <v>543</v>
       </c>
       <c r="D238">
-        <v>27.43019</v>
+        <v>27.588472199999998</v>
       </c>
       <c r="E238">
-        <v>94.738600000000005</v>
+        <v>94.723416700000001</v>
       </c>
       <c r="F238">
         <v>787059</v>
@@ -6939,10 +6909,10 @@
         <v>544</v>
       </c>
       <c r="D239">
-        <v>27.662458999999998</v>
+        <v>27.566417000000001</v>
       </c>
       <c r="E239">
-        <v>95.530233999999993</v>
+        <v>95.555165000000002</v>
       </c>
       <c r="F239">
         <v>786151</v>
@@ -6959,10 +6929,10 @@
         <v>545</v>
       </c>
       <c r="D240">
-        <v>27.22486</v>
+        <v>27.085699999999999</v>
       </c>
       <c r="E240">
-        <v>95.115740000000002</v>
+        <v>95.170100000000005</v>
       </c>
       <c r="F240">
         <v>785693</v>
@@ -6979,10 +6949,10 @@
         <v>546</v>
       </c>
       <c r="D241">
-        <v>28.57808</v>
+        <v>27.192900000000002</v>
       </c>
       <c r="E241">
-        <v>77.172709999999995</v>
+        <v>94.091899999999995</v>
       </c>
       <c r="F241">
         <v>787032</v>
@@ -6999,10 +6969,10 @@
         <v>547</v>
       </c>
       <c r="D242">
-        <v>26.672872999999999</v>
+        <v>24.151800000000001</v>
       </c>
       <c r="E242">
-        <v>94.105331000000007</v>
+        <v>92.181700000000006</v>
       </c>
       <c r="F242">
         <v>785616</v>
@@ -7019,10 +6989,10 @@
         <v>548</v>
       </c>
       <c r="D243">
-        <v>26.592099999999999</v>
+        <v>26.4008</v>
       </c>
       <c r="E243">
-        <v>93.849410000000006</v>
+        <v>93.483400000000003</v>
       </c>
       <c r="F243">
         <v>785611</v>
@@ -7039,10 +7009,10 @@
         <v>549</v>
       </c>
       <c r="D244">
-        <v>27.058523000000001</v>
+        <v>26.1234</v>
       </c>
       <c r="E244">
-        <v>95.080691999999999</v>
+        <v>91.123400000000004</v>
       </c>
       <c r="F244">
         <v>785691</v>
@@ -7059,10 +7029,10 @@
         <v>550</v>
       </c>
       <c r="D245">
-        <v>26.73732</v>
+        <v>26.710899999999999</v>
       </c>
       <c r="E245">
-        <v>93.198053000000002</v>
+        <v>93.172250000000005</v>
       </c>
       <c r="F245">
         <v>784176</v>
@@ -7099,10 +7069,10 @@
         <v>552</v>
       </c>
       <c r="D247">
-        <v>26.2957</v>
+        <v>27.448583299999999</v>
       </c>
       <c r="E247">
-        <v>93.860500000000002</v>
+        <v>94.891916699999996</v>
       </c>
       <c r="F247">
         <v>786004</v>
@@ -7119,10 +7089,10 @@
         <v>553</v>
       </c>
       <c r="D248">
-        <v>27.522808000000001</v>
+        <v>27.2746</v>
       </c>
       <c r="E248">
-        <v>94.883184999999997</v>
+        <v>95.070599999999999</v>
       </c>
       <c r="F248">
         <v>786001</v>
@@ -7139,10 +7109,10 @@
         <v>554</v>
       </c>
       <c r="D249">
-        <v>27.522808000000001</v>
+        <v>27.2746</v>
       </c>
       <c r="E249">
-        <v>94.883184999999997</v>
+        <v>95.070599999999999</v>
       </c>
       <c r="F249">
         <v>786001</v>
@@ -7159,10 +7129,10 @@
         <v>555</v>
       </c>
       <c r="D250">
-        <v>28.577559999999998</v>
+        <v>27.253399999999999</v>
       </c>
       <c r="E250">
-        <v>77.171559999999999</v>
+        <v>95.392200000000003</v>
       </c>
       <c r="F250">
         <v>786171</v>
@@ -7179,10 +7149,10 @@
         <v>556</v>
       </c>
       <c r="D251">
-        <v>27.344408000000001</v>
+        <v>27.479861100000001</v>
       </c>
       <c r="E251">
-        <v>95.278892999999997</v>
+        <v>94.905500000000004</v>
       </c>
       <c r="F251">
         <v>786602</v>
@@ -7199,10 +7169,10 @@
         <v>557</v>
       </c>
       <c r="D252">
-        <v>27.435870000000001</v>
+        <v>27.463888900000001</v>
       </c>
       <c r="E252">
-        <v>95.026989999999998</v>
+        <v>95.079916699999998</v>
       </c>
       <c r="F252">
         <v>786101</v>
@@ -7219,10 +7189,10 @@
         <v>558</v>
       </c>
       <c r="D253">
-        <v>27.43019</v>
+        <v>27.480789000000001</v>
       </c>
       <c r="E253">
-        <v>94.738600000000005</v>
+        <v>94.556648999999993</v>
       </c>
       <c r="F253">
         <v>787057</v>
@@ -7239,10 +7209,10 @@
         <v>559</v>
       </c>
       <c r="D254">
-        <v>26.822130000000001</v>
+        <v>26.273900000000001</v>
       </c>
       <c r="E254">
-        <v>94.815269999999998</v>
+        <v>94.012</v>
       </c>
       <c r="F254">
         <v>785610</v>
@@ -7259,10 +7229,10 @@
         <v>560</v>
       </c>
       <c r="D255">
-        <v>27.40652</v>
+        <v>27.254000000000001</v>
       </c>
       <c r="E255">
-        <v>94.343609999999998</v>
+        <v>94.190200000000004</v>
       </c>
       <c r="F255">
         <v>787034</v>
@@ -7279,10 +7249,10 @@
         <v>561</v>
       </c>
       <c r="D256">
-        <v>26.773109999999999</v>
+        <v>26.758027800000001</v>
       </c>
       <c r="E256">
-        <v>94.213120000000004</v>
+        <v>94.210055600000004</v>
       </c>
       <c r="F256">
         <v>785001</v>
@@ -7299,10 +7269,10 @@
         <v>562</v>
       </c>
       <c r="D257">
-        <v>27.279430000000001</v>
+        <v>27.145</v>
       </c>
       <c r="E257">
-        <v>94.905069999999995</v>
+        <v>94.531800000000004</v>
       </c>
       <c r="F257">
         <v>785675</v>
@@ -7339,10 +7309,10 @@
         <v>564</v>
       </c>
       <c r="D259">
-        <v>27.28</v>
+        <v>27.1738</v>
       </c>
       <c r="E259">
-        <v>94.09</v>
+        <v>94.0548</v>
       </c>
       <c r="F259">
         <v>787051</v>
@@ -7419,10 +7389,10 @@
         <v>568</v>
       </c>
       <c r="D263">
-        <v>27.48</v>
+        <v>27.4868056</v>
       </c>
       <c r="E263">
-        <v>95.43</v>
+        <v>95.437555599999996</v>
       </c>
       <c r="F263">
         <v>786170</v>
@@ -7439,10 +7409,10 @@
         <v>569</v>
       </c>
       <c r="D264">
-        <v>27.29</v>
+        <v>27.287444399999998</v>
       </c>
       <c r="E264">
-        <v>95.66</v>
+        <v>95.669972200000004</v>
       </c>
       <c r="F264">
         <v>786181</v>
@@ -7579,10 +7549,10 @@
         <v>575</v>
       </c>
       <c r="D271">
-        <v>27.291499999999999</v>
+        <v>27.492190999999998</v>
       </c>
       <c r="E271">
-        <v>95.212000000000003</v>
+        <v>95.346774999999994</v>
       </c>
       <c r="F271">
         <v>786125</v>
@@ -7599,10 +7569,10 @@
         <v>576</v>
       </c>
       <c r="D272">
-        <v>27.49</v>
+        <v>27.494555600000002</v>
       </c>
       <c r="E272">
-        <v>95.25</v>
+        <v>95.254861099999999</v>
       </c>
       <c r="F272">
         <v>786183</v>
@@ -7619,10 +7589,10 @@
         <v>577</v>
       </c>
       <c r="D273">
-        <v>26.709250000000001</v>
+        <v>26.432300000000001</v>
       </c>
       <c r="E273">
-        <v>93.975111100000007</v>
+        <v>93.585700000000003</v>
       </c>
       <c r="F273">
         <v>785614</v>
@@ -7679,10 +7649,10 @@
         <v>579</v>
       </c>
       <c r="D276">
-        <v>27.71</v>
+        <v>27.480499999999999</v>
       </c>
       <c r="E276">
-        <v>94.88</v>
+        <v>94.959500000000006</v>
       </c>
       <c r="F276">
         <v>787061</v>
@@ -7702,7 +7672,7 @@
         <v>27.28</v>
       </c>
       <c r="E277">
-        <v>95.19</v>
+        <v>95.194999999999993</v>
       </c>
       <c r="F277">
         <v>786145</v>
@@ -7773,10 +7743,10 @@
         <v>584</v>
       </c>
       <c r="D281">
-        <v>27.71</v>
+        <v>27.480499999999999</v>
       </c>
       <c r="E281">
-        <v>94.88</v>
+        <v>94.959500000000006</v>
       </c>
       <c r="F281">
         <v>787061</v>
@@ -7793,10 +7763,10 @@
         <v>585</v>
       </c>
       <c r="D282">
-        <v>27.291499999999999</v>
+        <v>27.492190999999998</v>
       </c>
       <c r="E282">
-        <v>95.212000000000003</v>
+        <v>95.346774999999994</v>
       </c>
       <c r="F282">
         <v>786125</v>
@@ -7829,6 +7799,9 @@
       <c r="B284" t="s">
         <v>308</v>
       </c>
+      <c r="F284">
+        <v>0</v>
+      </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
@@ -7837,6 +7810,9 @@
       <c r="B285" t="s">
         <v>308</v>
       </c>
+      <c r="F285">
+        <v>0</v>
+      </c>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
@@ -7845,6 +7821,9 @@
       <c r="B286" t="s">
         <v>308</v>
       </c>
+      <c r="F286">
+        <v>0</v>
+      </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
@@ -7853,6 +7832,9 @@
       <c r="B287" t="s">
         <v>308</v>
       </c>
+      <c r="F287">
+        <v>0</v>
+      </c>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
@@ -7861,85 +7843,118 @@
       <c r="B288" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F288">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>293</v>
       </c>
       <c r="B289" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F289">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>294</v>
       </c>
       <c r="B290" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>295</v>
       </c>
       <c r="B291" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F291">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>296</v>
       </c>
       <c r="B292" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F292">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>297</v>
       </c>
       <c r="B293" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F293">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>298</v>
       </c>
       <c r="B294" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F294">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>299</v>
       </c>
       <c r="B295" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>300</v>
       </c>
       <c r="B296" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>301</v>
       </c>
       <c r="B297" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F297">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>302</v>
       </c>
       <c r="B298" t="s">
         <v>308</v>
+      </c>
+      <c r="F298">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>